<commit_message>
Using Data Providers and getting data from excel
</commit_message>
<xml_diff>
--- a/src/test/resources/com/liveproject/excel/testData.xlsx
+++ b/src/test/resources/com/liveproject/excel/testData.xlsx
@@ -3,8 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="AddCustomerTest" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="OpenAccountTest" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="CreateAccountTest" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="LoginTest" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="test-suite" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
@@ -13,88 +13,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
-  <si>
-    <t>firstName</t>
-  </si>
-  <si>
-    <t>customerName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>TCID</t>
   </si>
   <si>
-    <t>lastName</t>
-  </si>
-  <si>
-    <t>postCode</t>
-  </si>
-  <si>
-    <t>alertText</t>
-  </si>
-  <si>
-    <t>runmode</t>
-  </si>
-  <si>
-    <t>currency</t>
-  </si>
-  <si>
-    <t>Divya G</t>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>accountName</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
   <si>
     <t>Divya</t>
   </si>
   <si>
-    <t>Dollar</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>Runmode</t>
-  </si>
-  <si>
-    <t>BankManagerLoginTest</t>
-  </si>
-  <si>
-    <t>1234</t>
+    <t>LoginTest</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>Customer added successfully</t>
-  </si>
-  <si>
-    <t>AddCustomerTest</t>
-  </si>
-  <si>
-    <t>OpenAccountTest</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Aditya</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>344</t>
-  </si>
-  <si>
-    <t>Navya</t>
-  </si>
-  <si>
-    <t>324</t>
+    <t>CreateAccountTest</t>
+  </si>
+  <si>
+    <t>g.divya.us@gmail.com</t>
+  </si>
+  <si>
+    <t>Munnig25</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -102,9 +60,6 @@
     </font>
     <font>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <name val="Arial"/>
     </font>
     <font/>
@@ -117,35 +72,20 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <right/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -374,70 +314,12 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -456,19 +338,25 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -487,35 +375,27 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>19</v>
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>